<commit_message>
Ticket ID : SAW-431 Description : SAW should support ACL service as a part of security features - Maria DB changes
</commit_message>
<xml_diff>
--- a/Database/Source/Data_Entry_Automation/table_structure_mapping.xlsx
+++ b/Database/Source/Data_Entry_Automation/table_structure_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Product_Wise_Script\SAW\Data_Entry_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Product_Wise_Script\SAW\1.1.0.0\Database\Source\Data_Entry_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="116">
   <si>
     <t>Table Name</t>
   </si>
@@ -359,10 +359,19 @@
     <t>ROLE_CODE</t>
   </si>
   <si>
-    <t>W6ph5Mm5Pz8GgiULbPgzG37mj9g=</t>
-  </si>
-  <si>
     <t>PWD_MODIFIED_DATE</t>
+  </si>
+  <si>
+    <t>MODULE_URL</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>RsjpEvOkJwdvnSkVcGoIUwpXNIw=</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -419,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -428,6 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K164"/>
+  <dimension ref="A1:K167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D113" workbookViewId="0">
-      <selection activeCell="K133" sqref="K133"/>
+    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,20 +1780,18 @@
         <v>38</v>
       </c>
       <c r="E38" s="2"/>
-      <c r="F38" s="2">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" s="2">
         <v>1</v>
       </c>
-      <c r="K38" s="2"/>
+      <c r="K38" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -2427,17 +2435,17 @@
         <v>46</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" s="2"/>
     </row>
@@ -2452,23 +2460,19 @@
         <v>46</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2">
-        <v>1</v>
-      </c>
-      <c r="I63" s="2">
-        <v>0</v>
-      </c>
-      <c r="J63" s="2">
-        <v>1</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="H63" s="2"/>
+      <c r="I63" s="4">
+        <v>1</v>
+      </c>
+      <c r="J63" s="4">
+        <v>1</v>
+      </c>
+      <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -2481,23 +2485,19 @@
         <v>46</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2">
-        <v>1</v>
-      </c>
-      <c r="I64" s="2">
-        <v>0</v>
-      </c>
-      <c r="J64" s="2">
-        <v>1</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="H64" s="2"/>
+      <c r="I64" s="4">
+        <v>1</v>
+      </c>
+      <c r="J64" s="4">
+        <v>1</v>
+      </c>
+      <c r="K64" s="2"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
@@ -2510,7 +2510,7 @@
         <v>46</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -2522,9 +2522,11 @@
         <v>0</v>
       </c>
       <c r="J65" s="2">
-        <v>0</v>
-      </c>
-      <c r="K65" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
@@ -2537,7 +2539,7 @@
         <v>46</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -2549,9 +2551,11 @@
         <v>0</v>
       </c>
       <c r="J66" s="2">
-        <v>0</v>
-      </c>
-      <c r="K66" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
@@ -2564,7 +2568,7 @@
         <v>46</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -2591,7 +2595,7 @@
         <v>46</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -2609,57 +2613,55 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E69" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="4">
-        <v>0</v>
-      </c>
-      <c r="J69" s="4">
+      <c r="H69" s="2">
+        <v>1</v>
+      </c>
+      <c r="I69" s="2">
+        <v>0</v>
+      </c>
+      <c r="J69" s="2">
         <v>0</v>
       </c>
       <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E70" s="2"/>
-      <c r="F70" s="2">
-        <v>1</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H70" s="2"/>
-      <c r="I70" s="4">
-        <v>1</v>
-      </c>
-      <c r="J70" s="4">
-        <v>1</v>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2">
+        <v>1</v>
+      </c>
+      <c r="I70" s="2">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2">
+        <v>0</v>
       </c>
       <c r="K70" s="2"/>
     </row>
@@ -2674,17 +2676,19 @@
         <v>49</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E71" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1</v>
+      </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J71" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71" s="2"/>
     </row>
@@ -2699,11 +2703,15 @@
         <v>49</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H72" s="2"/>
       <c r="I72" s="4">
         <v>1</v>
@@ -2724,7 +2732,7 @@
         <v>49</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2749,7 +2757,7 @@
         <v>49</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2774,7 +2782,7 @@
         <v>49</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -2799,23 +2807,19 @@
         <v>49</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2">
-        <v>1</v>
-      </c>
-      <c r="I76" s="2">
-        <v>0</v>
-      </c>
-      <c r="J76" s="2">
-        <v>1</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="H76" s="2"/>
+      <c r="I76" s="4">
+        <v>1</v>
+      </c>
+      <c r="J76" s="4">
+        <v>1</v>
+      </c>
+      <c r="K76" s="2"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
@@ -2828,23 +2832,19 @@
         <v>49</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="2">
-        <v>1</v>
-      </c>
-      <c r="I77" s="2">
-        <v>0</v>
-      </c>
-      <c r="J77" s="2">
-        <v>1</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="H77" s="2"/>
+      <c r="I77" s="4">
+        <v>1</v>
+      </c>
+      <c r="J77" s="4">
+        <v>1</v>
+      </c>
+      <c r="K77" s="2"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
@@ -2857,18 +2857,16 @@
         <v>49</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="2">
-        <v>1</v>
-      </c>
-      <c r="I78" s="2">
-        <v>0</v>
-      </c>
-      <c r="J78" s="2">
+      <c r="H78" s="2"/>
+      <c r="I78" s="4">
+        <v>0</v>
+      </c>
+      <c r="J78" s="4">
         <v>0</v>
       </c>
       <c r="K78" s="2"/>
@@ -2884,7 +2882,7 @@
         <v>49</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -2896,9 +2894,11 @@
         <v>0</v>
       </c>
       <c r="J79" s="2">
-        <v>0</v>
-      </c>
-      <c r="K79" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
@@ -2911,7 +2911,7 @@
         <v>49</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -2923,9 +2923,11 @@
         <v>0</v>
       </c>
       <c r="J80" s="2">
-        <v>0</v>
-      </c>
-      <c r="K80" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
@@ -2938,7 +2940,7 @@
         <v>49</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -2956,82 +2958,82 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E82" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="4">
-        <v>0</v>
-      </c>
-      <c r="J82" s="4">
+      <c r="H82" s="2">
+        <v>1</v>
+      </c>
+      <c r="I82" s="2">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2">
         <v>0</v>
       </c>
       <c r="K82" s="2"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E83" s="2"/>
-      <c r="F83" s="2">
-        <v>1</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H83" s="2"/>
-      <c r="I83" s="4">
-        <v>1</v>
-      </c>
-      <c r="J83" s="4">
-        <v>1</v>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2">
+        <v>1</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2">
+        <v>0</v>
       </c>
       <c r="K83" s="2"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="4">
-        <v>1</v>
-      </c>
-      <c r="J84" s="4">
-        <v>1</v>
+      <c r="H84" s="2">
+        <v>1</v>
+      </c>
+      <c r="I84" s="2">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2">
+        <v>0</v>
       </c>
       <c r="K84" s="2"/>
     </row>
@@ -3046,17 +3048,19 @@
         <v>56</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E85" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J85" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K85" s="2"/>
     </row>
@@ -3071,11 +3075,15 @@
         <v>56</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
+      <c r="F86" s="2">
+        <v>1</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H86" s="2"/>
       <c r="I86" s="4">
         <v>1</v>
@@ -3096,7 +3104,7 @@
         <v>56</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
@@ -3121,7 +3129,7 @@
         <v>56</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -3146,7 +3154,7 @@
         <v>56</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -3171,23 +3179,19 @@
         <v>56</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="2">
-        <v>1</v>
-      </c>
-      <c r="I90" s="2">
-        <v>0</v>
-      </c>
-      <c r="J90" s="2">
-        <v>1</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="H90" s="2"/>
+      <c r="I90" s="4">
+        <v>1</v>
+      </c>
+      <c r="J90" s="4">
+        <v>1</v>
+      </c>
+      <c r="K90" s="2"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
@@ -3200,23 +3204,19 @@
         <v>56</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2">
-        <v>1</v>
-      </c>
-      <c r="I91" s="2">
-        <v>0</v>
-      </c>
-      <c r="J91" s="2">
-        <v>1</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="H91" s="2"/>
+      <c r="I91" s="4">
+        <v>1</v>
+      </c>
+      <c r="J91" s="4">
+        <v>1</v>
+      </c>
+      <c r="K91" s="2"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
@@ -3229,19 +3229,17 @@
         <v>56</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="2">
-        <v>1</v>
-      </c>
-      <c r="I92" s="2">
-        <v>0</v>
-      </c>
-      <c r="J92" s="2">
-        <v>0</v>
+      <c r="H92" s="2"/>
+      <c r="I92" s="4">
+        <v>1</v>
+      </c>
+      <c r="J92" s="4">
+        <v>1</v>
       </c>
       <c r="K92" s="2"/>
     </row>
@@ -3256,7 +3254,7 @@
         <v>56</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -3268,9 +3266,11 @@
         <v>0</v>
       </c>
       <c r="J93" s="2">
-        <v>0</v>
-      </c>
-      <c r="K93" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
@@ -3283,7 +3283,7 @@
         <v>56</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -3295,9 +3295,11 @@
         <v>0</v>
       </c>
       <c r="J94" s="2">
-        <v>0</v>
-      </c>
-      <c r="K94" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
@@ -3310,7 +3312,7 @@
         <v>56</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -3328,82 +3330,82 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E96" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="4">
-        <v>0</v>
-      </c>
-      <c r="J96" s="4">
+      <c r="H96" s="2">
+        <v>1</v>
+      </c>
+      <c r="I96" s="2">
+        <v>0</v>
+      </c>
+      <c r="J96" s="2">
         <v>0</v>
       </c>
       <c r="K96" s="2"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="E97" s="2"/>
-      <c r="F97" s="2">
-        <v>1</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H97" s="2"/>
-      <c r="I97" s="4">
-        <v>1</v>
-      </c>
-      <c r="J97" s="4">
-        <v>1</v>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2">
+        <v>1</v>
+      </c>
+      <c r="I97" s="2">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2">
+        <v>0</v>
       </c>
       <c r="K97" s="2"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="4">
-        <v>1</v>
-      </c>
-      <c r="J98" s="4">
-        <v>1</v>
+      <c r="H98" s="2">
+        <v>1</v>
+      </c>
+      <c r="I98" s="2">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2">
+        <v>0</v>
       </c>
       <c r="K98" s="2"/>
     </row>
@@ -3418,17 +3420,19 @@
         <v>62</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E99" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="E99" s="2">
+        <v>1</v>
+      </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J99" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K99" s="2"/>
     </row>
@@ -3443,11 +3447,15 @@
         <v>62</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
+      <c r="F100" s="2">
+        <v>1</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="H100" s="2"/>
       <c r="I100" s="4">
         <v>1</v>
@@ -3468,7 +3476,7 @@
         <v>62</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -3493,23 +3501,19 @@
         <v>62</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2">
-        <v>1</v>
-      </c>
-      <c r="I102" s="2">
-        <v>0</v>
-      </c>
-      <c r="J102" s="2">
-        <v>1</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="H102" s="2"/>
+      <c r="I102" s="4">
+        <v>1</v>
+      </c>
+      <c r="J102" s="4">
+        <v>1</v>
+      </c>
+      <c r="K102" s="2"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
@@ -3522,23 +3526,19 @@
         <v>62</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
-      <c r="H103" s="2">
-        <v>1</v>
-      </c>
-      <c r="I103" s="2">
-        <v>0</v>
-      </c>
-      <c r="J103" s="2">
-        <v>1</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="H103" s="2"/>
+      <c r="I103" s="4">
+        <v>1</v>
+      </c>
+      <c r="J103" s="4">
+        <v>1</v>
+      </c>
+      <c r="K103" s="2"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
@@ -3551,19 +3551,17 @@
         <v>62</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
-      <c r="H104" s="2">
-        <v>1</v>
-      </c>
-      <c r="I104" s="2">
-        <v>0</v>
-      </c>
-      <c r="J104" s="2">
-        <v>0</v>
+      <c r="H104" s="2"/>
+      <c r="I104" s="4">
+        <v>1</v>
+      </c>
+      <c r="J104" s="4">
+        <v>1</v>
       </c>
       <c r="K104" s="2"/>
     </row>
@@ -3578,7 +3576,7 @@
         <v>62</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -3590,9 +3588,11 @@
         <v>0</v>
       </c>
       <c r="J105" s="2">
-        <v>0</v>
-      </c>
-      <c r="K105" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
@@ -3605,7 +3605,7 @@
         <v>62</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -3617,9 +3617,11 @@
         <v>0</v>
       </c>
       <c r="J106" s="2">
-        <v>0</v>
-      </c>
-      <c r="K106" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
@@ -3632,7 +3634,7 @@
         <v>62</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -3650,23 +3652,23 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E108" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
+      <c r="H108" s="2">
+        <v>1</v>
+      </c>
       <c r="I108" s="2">
         <v>0</v>
       </c>
@@ -3677,59 +3679,55 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E109" s="2"/>
-      <c r="F109" s="2">
-        <v>1</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2">
+        <v>1</v>
+      </c>
       <c r="I109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K109" s="2"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="E110" s="2"/>
-      <c r="F110" s="2">
-        <v>1</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2">
+        <v>1</v>
+      </c>
       <c r="I110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J110" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K110" s="2"/>
     </row>
@@ -3744,17 +3742,19 @@
         <v>67</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E111" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="E111" s="2">
+        <v>1</v>
+      </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J111" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K111" s="2"/>
     </row>
@@ -3769,23 +3769,23 @@
         <v>67</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2">
-        <v>1</v>
-      </c>
+      <c r="F112" s="2">
+        <v>1</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H112" s="2"/>
       <c r="I112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J112" s="2">
         <v>1</v>
       </c>
-      <c r="K112" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="K112" s="2"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
@@ -3798,23 +3798,23 @@
         <v>67</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2">
-        <v>1</v>
-      </c>
+      <c r="F113" s="2">
+        <v>1</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H113" s="2"/>
       <c r="I113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J113" s="2">
         <v>1</v>
       </c>
-      <c r="K113" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="K113" s="2"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
@@ -3827,19 +3827,17 @@
         <v>67</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-      <c r="H114" s="2">
-        <v>1</v>
-      </c>
+      <c r="H114" s="2"/>
       <c r="I114" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J114" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K114" s="2"/>
     </row>
@@ -3854,7 +3852,7 @@
         <v>67</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -3866,9 +3864,11 @@
         <v>0</v>
       </c>
       <c r="J115" s="2">
-        <v>0</v>
-      </c>
-      <c r="K115" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
@@ -3881,7 +3881,7 @@
         <v>67</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -3893,9 +3893,11 @@
         <v>0</v>
       </c>
       <c r="J116" s="2">
-        <v>0</v>
-      </c>
-      <c r="K116" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
@@ -3908,7 +3910,7 @@
         <v>67</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -3926,23 +3928,23 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E118" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
+      <c r="H118" s="2">
+        <v>1</v>
+      </c>
       <c r="I118" s="2">
         <v>0</v>
       </c>
@@ -3953,55 +3955,55 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
+      <c r="H119" s="2">
+        <v>1</v>
+      </c>
       <c r="I119" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J119" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K119" s="2"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E120" s="2"/>
-      <c r="F120" s="2">
-        <v>1</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2">
+        <v>1</v>
+      </c>
       <c r="I120" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J120" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K120" s="2"/>
     </row>
@@ -4016,25 +4018,23 @@
         <v>71</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2">
-        <v>1</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E121" s="2">
+        <v>1</v>
+      </c>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J121" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>71</v>
       </c>
@@ -4045,21 +4045,19 @@
         <v>71</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J122" s="2">
         <v>1</v>
       </c>
-      <c r="K122" s="5" t="s">
-        <v>111</v>
-      </c>
+      <c r="K122" s="2"/>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
@@ -4072,11 +4070,15 @@
         <v>71</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
-      <c r="G123" s="2"/>
+      <c r="F123" s="2">
+        <v>1</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="H123" s="2"/>
       <c r="I123" s="2">
         <v>1</v>
@@ -4097,21 +4099,25 @@
         <v>71</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
+      <c r="F124" s="2">
+        <v>1</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H124" s="2"/>
       <c r="I124" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J124" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>71</v>
       </c>
@@ -4122,19 +4128,21 @@
         <v>71</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J125" s="2">
         <v>1</v>
       </c>
-      <c r="K125" s="2"/>
+      <c r="K125" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
@@ -4147,7 +4155,7 @@
         <v>71</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
@@ -4172,23 +4180,19 @@
         <v>71</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
-      <c r="H127" s="2">
-        <v>1</v>
-      </c>
+      <c r="H127" s="2"/>
       <c r="I127" s="2">
         <v>0</v>
       </c>
       <c r="J127" s="2">
-        <v>1</v>
-      </c>
-      <c r="K127" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K127" s="2"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
@@ -4201,23 +4205,19 @@
         <v>71</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
-      <c r="H128" s="2">
-        <v>1</v>
-      </c>
+      <c r="H128" s="2"/>
       <c r="I128" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J128" s="2">
         <v>1</v>
       </c>
-      <c r="K128" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="K128" s="2"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
@@ -4230,19 +4230,17 @@
         <v>71</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
-      <c r="H129" s="2">
-        <v>1</v>
-      </c>
+      <c r="H129" s="2"/>
       <c r="I129" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J129" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K129" s="2"/>
     </row>
@@ -4257,7 +4255,7 @@
         <v>71</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
@@ -4269,9 +4267,11 @@
         <v>0</v>
       </c>
       <c r="J130" s="2">
-        <v>0</v>
-      </c>
-      <c r="K130" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
@@ -4284,7 +4284,7 @@
         <v>71</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
@@ -4296,9 +4296,11 @@
         <v>0</v>
       </c>
       <c r="J131" s="2">
-        <v>0</v>
-      </c>
-      <c r="K131" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K131" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
@@ -4311,7 +4313,7 @@
         <v>71</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
@@ -4338,102 +4340,102 @@
         <v>71</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
+      <c r="H133" s="2">
+        <v>1</v>
+      </c>
       <c r="I133" s="2">
         <v>0</v>
       </c>
       <c r="J133" s="2">
-        <v>1</v>
-      </c>
-      <c r="K133" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K133" s="2"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E134" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="4">
-        <v>0</v>
-      </c>
-      <c r="J134" s="4">
+      <c r="H134" s="2">
+        <v>1</v>
+      </c>
+      <c r="I134" s="2">
+        <v>0</v>
+      </c>
+      <c r="J134" s="2">
         <v>0</v>
       </c>
       <c r="K134" s="2"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E135" s="2"/>
-      <c r="F135" s="2">
-        <v>1</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H135" s="2"/>
-      <c r="I135" s="4">
-        <v>1</v>
-      </c>
-      <c r="J135" s="4">
-        <v>1</v>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="2">
+        <v>1</v>
+      </c>
+      <c r="I135" s="2">
+        <v>0</v>
+      </c>
+      <c r="J135" s="2">
+        <v>0</v>
       </c>
       <c r="K135" s="2"/>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
-      <c r="I136" s="4">
-        <v>1</v>
-      </c>
-      <c r="J136" s="4">
-        <v>1</v>
-      </c>
-      <c r="K136" s="2"/>
+      <c r="I136" s="2">
+        <v>0</v>
+      </c>
+      <c r="J136" s="2">
+        <v>1</v>
+      </c>
+      <c r="K136" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
@@ -4446,17 +4448,19 @@
         <v>79</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E137" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="E137" s="2">
+        <v>1</v>
+      </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J137" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K137" s="2"/>
     </row>
@@ -4471,11 +4475,15 @@
         <v>79</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
-      <c r="G138" s="2"/>
+      <c r="F138" s="2">
+        <v>1</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H138" s="2"/>
       <c r="I138" s="4">
         <v>1</v>
@@ -4496,17 +4504,17 @@
         <v>79</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
       <c r="I139" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J139" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K139" s="2"/>
     </row>
@@ -4521,7 +4529,7 @@
         <v>79</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
@@ -4546,17 +4554,17 @@
         <v>79</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J141" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K141" s="2"/>
     </row>
@@ -4571,7 +4579,7 @@
         <v>79</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
@@ -4596,18 +4604,17 @@
         <v>79</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J143" s="4">
-        <f>-I1421</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K143" s="2"/>
     </row>
@@ -4622,17 +4629,17 @@
         <v>79</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
       <c r="I144" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J144" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K144" s="2"/>
     </row>
@@ -4647,7 +4654,7 @@
         <v>79</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
@@ -4672,7 +4679,7 @@
         <v>79</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
@@ -4682,6 +4689,7 @@
         <v>0</v>
       </c>
       <c r="J146" s="4">
+        <f>-I1424</f>
         <v>0</v>
       </c>
       <c r="K146" s="2"/>
@@ -4697,17 +4705,17 @@
         <v>79</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
       <c r="I147" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J147" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K147" s="2"/>
     </row>
@@ -4722,7 +4730,7 @@
         <v>79</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
@@ -4747,7 +4755,7 @@
         <v>79</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
@@ -4772,7 +4780,7 @@
         <v>79</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
@@ -4797,7 +4805,7 @@
         <v>79</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
@@ -4822,7 +4830,7 @@
         <v>79</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E152" s="2"/>
       <c r="F152" s="2"/>
@@ -4847,7 +4855,7 @@
         <v>79</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
@@ -4872,7 +4880,7 @@
         <v>79</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E154" s="2"/>
       <c r="F154" s="2"/>
@@ -4897,7 +4905,7 @@
         <v>79</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
@@ -4922,7 +4930,7 @@
         <v>79</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
@@ -4947,7 +4955,7 @@
         <v>79</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
@@ -4972,7 +4980,7 @@
         <v>79</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -4997,7 +5005,7 @@
         <v>79</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
@@ -5022,7 +5030,7 @@
         <v>79</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
@@ -5047,7 +5055,7 @@
         <v>79</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
@@ -5063,20 +5071,18 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E162" s="2">
-        <v>1</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
@@ -5090,61 +5096,138 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="E163" s="2"/>
-      <c r="F163" s="2">
-        <v>1</v>
-      </c>
-      <c r="G163" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
       <c r="H163" s="2"/>
       <c r="I163" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J163" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K163" s="2"/>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="E164" s="2"/>
-      <c r="F164" s="2">
-        <v>1</v>
-      </c>
-      <c r="G164" s="2" t="s">
-        <v>79</v>
-      </c>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
       <c r="H164" s="2"/>
       <c r="I164" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J164" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K164" s="2"/>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E165" s="2">
+        <v>1</v>
+      </c>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="2"/>
+      <c r="I165" s="4">
+        <v>0</v>
+      </c>
+      <c r="J165" s="4">
+        <v>0</v>
+      </c>
+      <c r="K165" s="2"/>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2">
+        <v>1</v>
+      </c>
+      <c r="G166" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H166" s="2"/>
+      <c r="I166" s="4">
+        <v>1</v>
+      </c>
+      <c r="J166" s="4">
+        <v>1</v>
+      </c>
+      <c r="K166" s="2"/>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2">
+        <v>1</v>
+      </c>
+      <c r="G167" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H167" s="2"/>
+      <c r="I167" s="4">
+        <v>1</v>
+      </c>
+      <c r="J167" s="4">
+        <v>1</v>
+      </c>
+      <c r="K167" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>